<commit_message>
12051.1 2nd konkrete option, 2nd distractor
</commit_message>
<xml_diff>
--- a/hux2022/proverbs/items/GR1/itemtabelle_20220124(16.19)_ST.xlsx
+++ b/hux2022/proverbs/items/GR1/itemtabelle_20220124(16.19)_ST.xlsx
@@ -11,9 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="122">
-  <si>
-    <t>proverbs vorlagen</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="150">
+  <si>
+    <t>context2022</t>
+  </si>
+  <si>
+    <t>itemtabelle_20220129(13.51)_GR1</t>
   </si>
   <si>
     <t>item</t>
@@ -28,16 +31,22 @@
     <t>frage</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
+    <t>A1 figurativ, korrekt</t>
+  </si>
+  <si>
+    <t>A2 figurativ, inkorrekt</t>
+  </si>
+  <si>
+    <t>A3 konkret 1</t>
+  </si>
+  <si>
+    <t>A4 konkret 2</t>
+  </si>
+  <si>
+    <t>A5 Distraktor 1   (kontextgebunden)</t>
+  </si>
+  <si>
+    <t>A6 Distraktor 2   (kontextunabhängig, kein Name aus dem Kontext)</t>
   </si>
   <si>
     <t>comments</t>
@@ -49,28 +58,34 @@
     <t>Paul und Oskar sind gute Freunde und sprechen über Geld. Paul traut sich nicht, nach einer Lohnerhöhung zu fragen, weil ihr Chef gerade sehr gestresst ist und oft Leute anschreit. Paul fragt Oskar: Soll ich meinen Chef nach mehr Lohn fragen? Oskar antwortet: Hunde, die bellen, beißen nicht. Paul zu Oskar: Das ist richtig, dann sollte ich mutig sein.</t>
   </si>
   <si>
-    <t>Warum sagt Oskar: „Hunde die bellen, beißen nicht“ ?</t>
-  </si>
-  <si>
-    <t>Weil Oskar glaubt, dass Pauls Chef der Lohnerhöhung zustimmen wird.</t>
-  </si>
-  <si>
-    <t>Weil Oskar glaubt, Paul sollte mit der Frage warten, bis der Chef weniger Stress hat.</t>
-  </si>
-  <si>
-    <t>Weil Oskar glaubt, dass Paul von lauten Tieren nicht verletzt werden wird.</t>
+    <t>Warum sagt Oskar, Hunde die bellen, beißen nicht?</t>
+  </si>
+  <si>
+    <t>Weil Oskar glaubt, dass Pauls Vorgesetzter seinem Wunsch zustimmen wird.</t>
+  </si>
+  <si>
+    <t>Weil Oskar glaubt, Paul sollte mit der Frage warten, bis sein Vorgesetzter weniger Stress hat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weil Oskar glaubt, dass Paul von lauten Tieren nicht verletzt werden wird.   </t>
+  </si>
+  <si>
+    <t>Weil Vierbeiner ungefährlich werden, wenn sie zum Bellen ihre ganze Energie verbrauchen.</t>
   </si>
   <si>
     <t>Weil Oskar weiß, dass Paul den Joghurt aus dem Kühlschrank im Büro klaut.</t>
   </si>
   <si>
+    <t>Weil auf dem Parkplatz gerade zwei Autos zusammengestoßen sind.</t>
+  </si>
+  <si>
     <t>Wer im Glashaus sitzt soll nicht mit Steinen werfen</t>
   </si>
   <si>
     <t>Katja und Lulu sind miteinander befreundet und reden über ihrer Ehemänner. Katja überlegt, ihren zu Mann verlassen, weil er sie kürzlich betrogen hat. Katja fragt Lulu: Soll ich jetzt die Scheidung einreichen? Lulu antwortet: Wer im Glashaus sitzt, sollte nicht mit Steinen werfen. Katja antwortet: Ja, dann denke ich nochmal darüber nach.</t>
   </si>
   <si>
-    <t>Warum sagt Lulu „Wer im Glashaus sitzt, sollte nicht mit Steinen werfen“?</t>
+    <t>Warum sagt Lulu, wer im Glashaus sitzt, sollte nicht mit Steinen werfen?</t>
   </si>
   <si>
     <t>Weil Lulu weiß, dass Katja ihren Mann ebenfalls betrogen hat.</t>
@@ -82,7 +97,13 @@
     <t>Weil Lulu nicht möchte, dass Katja die Scheiben kaputt macht.</t>
   </si>
   <si>
-    <t>Weil Lulu möchte, dass Katja ihr einen Wellensittich schenkt.</t>
+    <t>Weil Lulu weiß, dass Katja nicht gut zielen kann.   Weil Katja sich  einem zerbrechlichen Gebäude befindet.</t>
+  </si>
+  <si>
+    <t>Weil in der Ehe oft mit Gegenständen geworfen wird.</t>
+  </si>
+  <si>
+    <t>Weil jemand bei Rot über die Ampel gefahren ist.</t>
   </si>
   <si>
     <t>Steter Tropfen höhlt den Stein</t>
@@ -91,7 +112,7 @@
     <t>Tom und Anna haben beide Klavierunterricht und lernen gerade das gleiche Musikstück. Tom spielt es aber nicht so gut wie Anna, weil er nicht so viel übt wie sie. Tom sagt zu Anna: Das Klavierstück werde ich niemals so gut spielen wie du. Anna antwortet: Steter Tropfen höhlt den Stein. Tom sagt darauf: Ja, das ist richtig.</t>
   </si>
   <si>
-    <t>Warum sagt Anna: Steter Tropfen höhlt den Stein?</t>
+    <t>Warum sagt Anna, Steter Tropfen höhlt den Stein?</t>
   </si>
   <si>
     <t>Weil Anna glaubt, dass Tom sich mehr anstrengen sollte.</t>
@@ -103,16 +124,22 @@
     <t>Weil Anna glaubt, dass Tom undicht wird.</t>
   </si>
   <si>
+    <t xml:space="preserve">Weil Tom ein Fels ist. </t>
+  </si>
+  <si>
     <t>Weil Anna glaubt, dass das Orchester im nächsten Jahr auf Tournee gehen wird.</t>
   </si>
   <si>
+    <t>Weil im Zoo das Affenhaus im Winter geschlossen ist.</t>
+  </si>
+  <si>
     <t>Die dümmsten Bauern ernten die dicksten Kartoffeln</t>
   </si>
   <si>
     <t>Sven und Karla arbeiten in einer Firma und unterhalten sich über ihren Kollegen Andreas. Andreas ist faul und überlässt seine Arbeit gerne anderen. Heute hat Andreas gekündigt, weil er eine Million Euro in der Lotterie gewonnen hat. Sven sagt zu Karla: Es ist kaum zu glauben, dass ausgerechnet Andreas soviel Glück hatte, oder? Karla antwortet: Die dümmsten Bauern ernten die dicksten Kartoffeln. Sven sagt: Ja, das hat sich wieder einmal bestätigt.</t>
   </si>
   <si>
-    <t>Warum sagt Karla: „Die dümmsten Bauern ernten die dicksten Kartoffeln“?</t>
+    <t>Warum sagt Karla, die dümmsten Bauern ernten die dicksten Kartoffeln?</t>
   </si>
   <si>
     <t>Weil Karla glaubt, dass Andreas das Geld nicht verdient hat.</t>
@@ -124,7 +151,13 @@
     <t>Weil Karla glaubt, dass Andreas ein Landwirt ist.</t>
   </si>
   <si>
-    <t>Weil Karla möchte, dass Andreas Püree für sie kocht.</t>
+    <t>Weil Andreas riesige Erdäpfel anbaut.</t>
+  </si>
+  <si>
+    <t>Weil die Reparatur des Traktors sehr teuer war.</t>
+  </si>
+  <si>
+    <t>Weil diese Woche Haferflocken  im Sonderangebot sind.</t>
   </si>
   <si>
     <t>Wenn die Katze aus dem Haus ist, tanzen die Mäuse auf dem Tisch.</t>
@@ -133,17 +166,22 @@
     <t>Die Eltern von Max und Moritz sind übers Wochenende weggefahren. Immer wenn die Eltern weg sind, kommen abends Oma und Opa vorbei, um Max und Moritz ins Bett zu bringen. Als Oma und Opa kommen, liegen Max und Moritz auf dem Sofa, essen Süßigkeiten und gucken Fernsehen. Oma: „Na sowas! Um diese Uhrzeit dürfen die Jungs doch kein Fernsehen mehr gucken.“ Opa: „Ja, das stimmt. Wenn die Katze aus dem Haus, tanzen die Mäuse auf dem Tisch.“ Oma: „Das kann man wohl sagen!“</t>
   </si>
   <si>
-    <t>Warum sagt Opa: „Wenn die Katze aus dem Haus ist, tanzen die Mäuse auf dem Tisch“?</t>
+    <t>Warum sagt Opa, Wenn die Katze aus dem Haus ist, tanzen die Mäuse auf dem Tisch“?</t>
   </si>
   <si>
     <t>Weil Max und Moritz sich nicht an die Regeln halten, wenn die Eltern nicht da sind.</t>
   </si>
   <si>
-    <t xml:space="preserve">Weil Max und Moritz sich an die Regeln halten, wenn die Eltern nicht da sind.
-</t>
-  </si>
-  <si>
-    <t>Weil Opa glaubt, dass die Mäuse auf dem Tisch herumlaufen, weil die Katze draußen ist.</t>
+    <t>Weil Max und Moritz sich ordentlich benehmen, wenn die Eltern nicht da sind.</t>
+  </si>
+  <si>
+    <t>Weil Opa glaubt, dass Mäuse auf dem Tisch herumlaufen, weil die Katze draußen ist.   Ohne clanging: Weil Opa glaubt, dass die Tiere dann auf den Möbeln herumspringen.</t>
+  </si>
+  <si>
+    <t>Weil Opa beobachtet hat, dass kleine Tiere von großen gejagt werden.</t>
+  </si>
+  <si>
+    <t>Weil Opa gerne Süßigkeiten essen möchte.</t>
   </si>
   <si>
     <t>Weil Opa noch nichts zum Abendbrot gegessen hat und hungrig ist.</t>
@@ -152,22 +190,22 @@
     <t>Eine Krähe hackt der anderen kein Auge aus.</t>
   </si>
   <si>
-    <t>Auf der Arbeit im Pausenraum ist die neue Kaffeemaschine kaputt gegangen. Der Chef verspricht eine große Belohnung für die Person, die ihm erzählt wem die Kaffeemaschine kaputt gegangen ist. ***A:*** “Glaubst du jemand wird zum Chef gehen und verraten wer es war?” ***B:*** “Auf keinen Fall. Eine Krähe hackt der anderen doch kein Auge aus.” ***A:*** “Ja, das denke ich auch.”</t>
-  </si>
-  <si>
-    <t>Warum sagt ***B:*** „Eine Krähe hackt der anderen doch kein Auge aus.“?</t>
-  </si>
-  <si>
-    <t>Weil ***B*** glaubt, dass die Arbeiter zusammenhalten und sich nicht gegenseitig beim Chef verraten.</t>
-  </si>
-  <si>
-    <t>Weil ***B*** denkt, dass die Arbeiter nicht zusammenhalten und sich gegenseitig beim Chef verraten würden.</t>
-  </si>
-  <si>
-    <t>Weil ***B*** weiß, dass Krähen friedlich miteinander umgehen.</t>
-  </si>
-  <si>
-    <t>Weil ***B*** weiß, dass ***A*** heute Spätschicht hat und noch lange bei der Arbeit sein wird.</t>
+    <t>Auf der Arbeit im Pausenraum ist die neue Kaffeemaschine kaputt gegangen. Die Chefin verspricht eine große Belohnung für die Person, die ihr erzählt wem die Kaffeemaschine kaputt gegangen ist. Sabine: “Glaubst du jemand wird zur Chefin gehen und verraten wer es war?” Paul: “Auf keinen Fall. Eine Krähe hackt der anderen doch kein Auge aus.” Sabine: “Hm, da bin ich mir nicht so sicher.”</t>
+  </si>
+  <si>
+    <t>Warum sagt Paul, Eine Krähe hackt der anderen doch kein Auge aus?</t>
+  </si>
+  <si>
+    <t>Weil Paul glaubt, dass die Arbeiter zusammenhalten und sich nicht gegenseitig bei ihrem Vorgesetzten verraten.</t>
+  </si>
+  <si>
+    <t>Weil Paul denkt, dass die Arbeiter nicht zusammenhalten und sich gegenseitig verraten würden.</t>
+  </si>
+  <si>
+    <t>Weil Paul weiß, dass Vögel friedlich miteinander umgehen.</t>
+  </si>
+  <si>
+    <t>Weil Paul weiß, dass Sabine heute Spätschicht hat und noch lange bei der Arbeit sein wird.</t>
   </si>
   <si>
     <t>Wenn das Kind ertrunken ist, deckt man den Brunnen zu.</t>
@@ -176,7 +214,7 @@
     <t>***A*** und ***B*** spazieren durchs Dorf und unterhalten sich. An der alten Straßenkreuzung bleiben sie stehen und schauen sich die neu gebaute Ampel an. ***A:***” Schade das die Ampel letzten Monat noch nicht da war, das hätte den Autounfall bestimmt verhindert.” ***B:*** “Das stimmt, erst wenn das Kind ertrunken ist, deckt man den Brunnen zu.” ***A:*** “Ja, leider”.</t>
   </si>
   <si>
-    <t>Warum sagt ***B:*** “Erst wenn das Kind ertrunken ist, deckt man den Brunnen zu.”?</t>
+    <t>Warum sagt ***B:***, Erst wenn das Kind ertrunken ist, deckt man den Brunnen zu?</t>
   </si>
   <si>
     <t>Weil die Kreuzung erst sicher gemacht wurde, nachdem der Unfall passiert ist.</t>
@@ -194,10 +232,10 @@
     <t>Wer anderen eine Grube gräbt, fällt selbst hinein.</t>
   </si>
   <si>
-    <t>***A*** will seiner Schwester ***B*** ein Bein stellen. Doch als er es machen will gerät er aus dem Gleichgewicht und fällt selbst auf den Boden. *A:* “Oh man, wie konnte das nur passieren." ***B:*** ”Tja, wer anderen eine Grube gräbt, fällt selbst hinein.” ***A:*** ”Ja, aber wirklich.”</t>
-  </si>
-  <si>
-    <t>Warum sagt ***B:*** “Wer anderen eine Grube gräbt, fällt selbst hinein.”?</t>
+    <t>***A*** will seiner Schwester ***B*** ein Bein stellen. Doch als er es machen will gerät er aus dem Gleichgewicht und fällt selbst auf den Boden. *A:* “Oh man, wie konnte das nur passieren. ***B:*** ”Tja, wer anderen eine Grube gräbt, fällt selbst hinein.” ***A:*** ”Ja, aber wirklich.”</t>
+  </si>
+  <si>
+    <t>Warum sagt ***B:***, wer anderen eine Grube gräbt, fällt selbst hinein?</t>
   </si>
   <si>
     <t>Weil ***B*** findet, dass ***A*** selber Schuld ist, dass er hingefallen ist.</t>
@@ -215,71 +253,88 @@
     <t>Geld regiert die Welt.</t>
   </si>
   <si>
-    <t>***A***: "Hast du das von dem reichen Bauern gehört, der angeblich unser Rathaus gekauft hat?" ***B***: "Nee. Aber würde mich nicht wundern." ***A***: "Wieso? Denkst du, die Stadt verkauft einfach so ihren Regierungssitz?" ***B***: "Na Geld regiert die Welt. ***A***: "Stimmt auch wieder."</t>
-  </si>
-  <si>
-    <t>Warum ist *Geld regiert die Welt* für Person *A* eine zufriedenstellende Antwort?</t>
-  </si>
-  <si>
-    <t>Weil auch *A* denkt, dass  der Stadt die Millionen wichtiger sind, als unabhängig zu bleiben.</t>
-  </si>
-  <si>
-    <t>Weil *A* denkt, dass die Stadt sich nicht so leicht kaufen lässt.</t>
-  </si>
-  <si>
-    <t>Weil *A* der Meinung ist, dass man sich eben für genug Geld durchaus ein Rathaus leisten kann.</t>
-  </si>
-  <si>
-    <t>Weil *A* denkt, dass der Bauer ein Kino aus dem Gebäude machen will.</t>
+    <t>***A*** und ***B*** unterhalten sich: ***A***: Hast du das von dem reichen Bauern gehört, der angeblich unser Rathaus gekauft hat? ***B***: Nee. Aber würde mich nicht wundern. ***A***: Wieso? Denkst du, die Stadt verkauft einfach so ihren Regierungssitz? ***B***: Na Geld regiert die Welt. ***A***: Stimmt auch wieder.</t>
+  </si>
+  <si>
+    <t>Warum ist *Geld regiert die Welt* für Person ***A*** eine zufriedenstellende Antwort?</t>
+  </si>
+  <si>
+    <t>Weil auch ***A*** denkt, dass der Stadt die Millionen wichtiger sind, als unabhängig zu bleiben.</t>
+  </si>
+  <si>
+    <t>Weil ***A*** denkt, dass der Stadt ihre Unabhängigkeit wichtiger als irgendwelche Millionen ist.</t>
+  </si>
+  <si>
+    <t>Weil ***A*** der Meinung ist, dass man sich eben mit genug Mitteln durchaus ein solches Haus leisten kann.</t>
+  </si>
+  <si>
+    <t>Weil ***A*** denkt, dass ein Stadtgebäude nicht so viel kostet.</t>
+  </si>
+  <si>
+    <t>Weil ***A*** denkt, dass der Unternehmer ein Kino aus dem Gebäude machen will.</t>
+  </si>
+  <si>
+    <t>Weil sie weiß, dass die Beleuchtung erst in der Dämmerung eingeschaltet wird.</t>
   </si>
   <si>
     <t>Unverhofft kommt oft.</t>
   </si>
   <si>
-    <t>Britta hat schon lange auf die Sonderauflage ihres Lieblingsbuches, Thomas Manns *Zauberberg*, gewartet. Als sie neulich zufällig an einer Buchhandlung vorbeigeht, sieht sie, wie die Verkäuferin gerade diese Sonderauflagen im Schaufenster verteilt. "Ha! Unverhofft kommt oft!" sagt sie zu sich selbst. Gerade hatte sie im Cafe, wo sie arbeitet, das Trinkgeld des ganzen Monats bekommen.</t>
-  </si>
-  <si>
-    <t>Warum entfährt ihr der Spruch *"Unverhofft kommt oft"?*</t>
-  </si>
-  <si>
-    <t>Weil sie gerade zufällig einen dicken Umschlag Geld in der Tasche hat?</t>
-  </si>
-  <si>
-    <t>Weil sie das ganze Geld für Kleinigkeiten ausgeben kann?</t>
-  </si>
-  <si>
-    <t>Weil sie in der Buchhandlung sehr häufig zu viel Geld ausgibt und sich darüber ärgert?</t>
+    <t>Britta hat schon lange auf die Sonderauflage ihres Lieblingsbuches, Thomas Manns *Zauberberg*, gewartet. Als sie neulich zufällig an einer Buchhandlung vorbeigeht, sieht sie, wie die Verkäuferin gerade diese Sonderauflagen im Schaufenster verteilt. Ha! Unverhofft kommt oft! sagt sie zu sich selbst. Gerade hatte sie im Cafe, wo sie arbeitet, das Trinkgeld des ganzen Monats bekommen.</t>
+  </si>
+  <si>
+    <t>Warum entfährt ihr der Spruch :Unverhofft kommt oft?:</t>
+  </si>
+  <si>
+    <t>Weil sie gerade zufällig einen dicken Umschlag Scheine in der Tasche hat, als sie an dem Laden vorbeigeht?</t>
+  </si>
+  <si>
+    <t>Weil sie die ganzen Scheine für Kleinigkeiten ausgeben kann?</t>
+  </si>
+  <si>
+    <t>Weil sie in dem Laden sehr häufig zu viel ausgibt und darauf gewartet hat, dass sich das ändert?</t>
+  </si>
+  <si>
+    <t>Weil in dem Laden ständig Ratgeberliteratur verkauft wird?</t>
   </si>
   <si>
     <t>Weil die Gäste im Cafe heute sehr geizig waren?</t>
   </si>
   <si>
+    <t>Weil auch Tunnel in anderen Gegenden gegraben werden?</t>
+  </si>
+  <si>
     <t>Je weniger man isst, desto länger ist man.</t>
   </si>
   <si>
-    <t>Mike ist ein leidenschaftlicher Koch in einem Restaurant. Trotzdem will er von den Speisen, die er zubereitet, nur wenig selbst essen. Als Suse ihn fragt, warum das so ist, antwortet er: "Na du weiszt, je weniger man isst, desto länger ist man." Suse sagt: "Okay, das verstehe ich. Ich dachte schon, dir schmecken deine Gerichte nicht."</t>
-  </si>
-  <si>
-    <t>Warum weisz Suse jetzt, dass Mike aus gesundheitlichen Gründen weniger essen möchte?</t>
-  </si>
-  <si>
-    <t>Weil Mike mit seiner Aussage zu verstehen gibt, länger leben zu wollen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weil Mike sein eigenes Essen zu gefährlich ist?
-</t>
-  </si>
-  <si>
-    <t>Weil Mike zugibt, Angst zu haben, durch zu wenig Essen zu lang und groß zu werden, um weiter in der engen Küche arbeiten zu können?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weil den Gästen die Eingangstür zum Restaurant zu klein ist. </t>
+    <t>Mike ist ein leidenschaftlicher Koch in einem Restaurant. Trotzdem will er von den Speisen, die er zubereitet, nur wenig selbst essen. Als Suse ihn fragt, warum das so ist, antwortet er: Na du weiszt, je weniger man isst, desto länger ist man. Suse sagt: Okay, das verstehe ich. Ich dachte schon, dir schmecken deine Gerichte nicht.</t>
+  </si>
+  <si>
+    <t>Warum weiß Suse jetzt, dass Mike aus gesundheitlichen Gründen weniger essen möchte?</t>
+  </si>
+  <si>
+    <t>Weil Mike mit seiner Aussage zu verstehen gibt, älter werden zu wollen.</t>
+  </si>
+  <si>
+    <t>Weil Mike seine Gerichte zu gefährlich sind?</t>
+  </si>
+  <si>
+    <t>Weil Mike damit zugibt, Angst zu haben, durch zu viel Nahrung zu groß zu werden, um weiter in der engen Küche arbeiten zu können?</t>
+  </si>
+  <si>
+    <t>Weil Mike einmal gesagt hat, dass er weniger zu sich nehmen möchte und das schon eine Weile her ist.</t>
+  </si>
+  <si>
+    <t>Weil den Gästen die Eingangstür zum Restaurant zu klein ist.</t>
+  </si>
+  <si>
+    <t>Weil er mit der S-Bahn direkt bis zum See fahren kann.</t>
   </si>
   <si>
     <t>Eine Schwalbe macht noch keinen Sommer.</t>
   </si>
   <si>
-    <t>Birgit und Karl sitzen in ihrer Laube. Sie haben gerade den Salat im Beet ausgepflanzt. Karl meint: "Und…, wie findest du's? Können wir bald ernten, oder?" Birgit überlegt kurz und sagt: "Na…, eine Schwalbe macht noch keinen Sommer." Karl antwortet: "Naja immerhin…, der Anfang ist gemacht."</t>
+    <t>Birgit und Karl sitzen in ihrer Laube. Sie haben gerade den Salat im Beet ausgepflanzt. Karl meint: Und…, wie findest du's? Können wir bald ernten, oder? Birgit überlegt kurz und sagt: Na…, eine Schwalbe macht noch keinen Sommer. Karl antwortet: Naja immerhin…, der Anfang ist gemacht.</t>
   </si>
   <si>
     <t>Warum sagt Birgit das mit der Schwalbe und dem Sommer?</t>
@@ -288,22 +343,28 @@
     <t>Weil sie denkt, dass bis man ernten kann, noch eine Menge zu tun sein wird.</t>
   </si>
   <si>
-    <t>Weil sie denkt, dass der Salat eh eingeht.</t>
-  </si>
-  <si>
-    <t>Weil sie denkt, dass die Vögel alles wegfressen werden.</t>
-  </si>
-  <si>
-    <t>Weil sie denkt, der Nachbar hat immer den grüneren Salat.</t>
+    <t>Weil sie denkt, dass sie sich jetzt ausruhen können.</t>
+  </si>
+  <si>
+    <t>Weil sie denkt, dass die Vögel in dieser Jahreszeit alles wegfressen werden.</t>
+  </si>
+  <si>
+    <t>Weil sie denkt, dass sie Vögel im letzten Winter kaum etwas zu fressen hatten.</t>
+  </si>
+  <si>
+    <t>Weil sie denkt, der Nachbar hat immer die grüneren Tomaten.</t>
+  </si>
+  <si>
+    <t>Weil sie denkt, dass der Badesee mitten im Wald liegt.</t>
   </si>
   <si>
     <t>Wie gewonnen, so zerronnen.</t>
   </si>
   <si>
-    <t>***A*** ist Schauspielerin und dreht gerade einen neuen Kinofilm. Sie erfährt, dass sie morgen nicht am Set gebraucht wird und einen freien Tag hat. ***A*** erhält am Abend einen Anruf von ***B***: Es gab Änderungen in der Tagesdisposition, sodass wir deine Szene vorziehen. Deine Calltime für morgen ist 06:30 Uhr. ***A*** antwortet: Wie gewonnen so zerronnen. ***B*** entgegnet ihr: Da hast du dich wohl zu früh gefreut. (Du weißt doch, wie es in diesem Business läuft)</t>
-  </si>
-  <si>
-    <t>Warum sagt ***A*** "wie gewonnen so zerronnen"?</t>
+    <t>***A*** ist Schauspielerin und dreht gerade einen neuen Kinofilm. Sie erfährt, dass sie morgen nicht am Set gebraucht wird und einen freien Tag hat. ***A*** erhält am Abend einen Anruf von ***B***: Es gab Änderungen in der Tagesdisposition, sodass wir deine Szene vorziehen. Deine Calltime für morgen ist 06:30 Uhr. ***A*** antwortet: Wie gewonnen so zerronnen. ***B*** entgegnet ihr: Da hast du dich wohl zu früh gefreut. Du weißt doch, wie es in diesem Business läuft.</t>
+  </si>
+  <si>
+    <t>Warum sagt ***A*** Wie gewonnen so zerronnen?</t>
   </si>
   <si>
     <t>Weil ***A*** glaubte frei zu haben und nun doch arbeiten gehen muss.</t>
@@ -312,31 +373,43 @@
     <t>Weil ***A*** frei hat und nicht arbeiten gehen muss.</t>
   </si>
   <si>
-    <t>Weil ***A***´s Preis/Sieg dahinschmilzt.</t>
+    <t>Weil ***A***´s Sieg dahinschmilzt.</t>
+  </si>
+  <si>
+    <t>Weil ***A*** ihren Lottoschein in der Waschmaschine gewaschen hat.</t>
   </si>
   <si>
     <t>Weil ***A*** Eis essen gehen möchte.</t>
   </si>
   <si>
+    <t>Weil ***A*** lieber Drachen fliegen lassen möchte.</t>
+  </si>
+  <si>
+    <t>stephan</t>
+  </si>
+  <si>
     <t>Es ist nicht alles Gold, was glänzt</t>
   </si>
   <si>
-    <t>A berichtet B von seinem erfolglosen Date (Verabredung) gestern Abend. Er hatte gehofft endlich seine Traumfrau gefunden zu haben. A sagt zu B: Wie kann man nur so wahnsinnig gut aussehen und doch so langweilig sein?! B antwortet A darauf: Es ist eben nicht alles Gold, was glänzt. A meint daraufhin: So könnte man es auch sagen.</t>
-  </si>
-  <si>
-    <t>Warum sagt B "es ist eben nicht alles Gold, was glänzt"?</t>
-  </si>
-  <si>
-    <t>Weil B meint, dass Attraktivität oft blenden (täuschen) kann.</t>
-  </si>
-  <si>
-    <t>Weil B findet, dass das äußere Erscheinungsbild den wahren Wert widerspeigelt.</t>
+    <t>***A*** berichtet ***B*** von seinem erfolglosen Date (Verabredung) gestern Abend. Er hatte gehofft endlich seine Traumfrau gefunden zu haben. ***A*** sagt zu ***B***: Wie kann man nur so wahnsinnig gut aussehen und doch so langweilig sein?! ***B*** antwortet ***A*** darauf: Es ist eben nicht alles Gold, was glänzt. ***A*** meint daraufhin: So könnte man es auch sagen.</t>
+  </si>
+  <si>
+    <t>Warum sagt ***B***, es ist eben nicht alles Gold, was glänzt?</t>
+  </si>
+  <si>
+    <t>Weil ***B*** meint, dass Attraktivität oft blenden (täuschen) kann.</t>
+  </si>
+  <si>
+    <t>Weil ***B*** findet, dass das äußere Erscheinungsbild den wahren Wert widerspeigelt.</t>
   </si>
   <si>
     <t>Weil das Bilnken (Schimmern) allein kein Charakteristkum (Alleinstellungsmerkmal) des Edelmetalls ist.</t>
   </si>
   <si>
-    <t>Weil B Lust auf ein Bad hat.</t>
+    <t>Weil ***B*** Lust auf ein Bad hat.</t>
+  </si>
+  <si>
+    <t>Dyke</t>
   </si>
   <si>
     <t>Der Klügere gibt nach.</t>
@@ -345,7 +418,7 @@
     <t>***A*** und ***B*** leben in einer Partnerschaft und diskutieren die Organisation der bevorstehenden Weihnachtsfeiertage. Beide haben ihren Eltern versprochen Heiligabend mit der Familien zu verbringen. ***A*** argumentiert: Wir waren letztes Jahr schon zu Besuch bei deinen Eltern. ***B*** entgegnet ihr daraufhin: Der Klügere muss wohl nachgeben. ***A*** sagt: Manchmal ist das wohl so.</t>
   </si>
   <si>
-    <t>Warum sagt ***B*** " der Klügere muss wohl nachgeben"?</t>
+    <t>Warum sagt ***B***, der Klügere muss wohl nachgeben?</t>
   </si>
   <si>
     <t>Weil ***B*** den Disput mit ***A*** beenden möchte.</t>
@@ -357,16 +430,25 @@
     <t>Weil ***B*** intelligenter ist als ***A***. (Weil ***B*** einen höheren IQ hat als ***A***)</t>
   </si>
   <si>
+    <t>Weil ***A*** ein dummer Mensch ist.</t>
+  </si>
+  <si>
     <t>Weil ***B*** mit ***A*** zu Abend essen möchte.</t>
   </si>
   <si>
-    <t>Spare dien Brot, so hast du in der Not.</t>
+    <t>Weil es heute noch regnen wird.</t>
+  </si>
+  <si>
+    <t>Claudia</t>
+  </si>
+  <si>
+    <t>Spare dein Brot, so hast du in der Not.</t>
   </si>
   <si>
     <t>Wie jeden Donnerstag ist ***A*** mit ***B*** zum Kaffeetrinken verabredet. ***A*** erzählt, dass sie auf dem Weg ihr Traumkleid in einem Schaufenster gesehen hat, sie sich das Kleid aber eigentlich nicht leisten kann. ***A*** fragt ***B***: Soll ich das Kleid kaufen, was meinst du? ***B*** antwortet: Spare dein Brot,so hast du in der Not. ***A*** sagt: Ja, vermutlich hast du recht.</t>
   </si>
   <si>
-    <t>Warum sagt ***B*** "Spare dein Brot, so hast du in der Not"?</t>
+    <t>Warum sagt ***B*** Spare dein Brot, so hast du in der Not?</t>
   </si>
   <si>
     <t>Weil ***B*** möchte, dass ***A*** ihr Geld für schlechte Zeiten bewahrt. (weil ***B*** nicht möchte, dass ***A*** ihr Geld unnötig ausgibt)</t>
@@ -545,51 +627,42 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1670,19 +1743,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:K23"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.4609" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.07812" style="1" customWidth="1"/>
-    <col min="4" max="11" width="16.3516" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52" style="1" customWidth="1"/>
+    <col min="3" max="3" width="166.672" style="1" customWidth="1"/>
+    <col min="4" max="4" width="68.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="101.172" style="1" customWidth="1"/>
+    <col min="6" max="6" width="72.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="129" style="1" customWidth="1"/>
+    <col min="8" max="8" width="80.3516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="69.1719" style="1" customWidth="1"/>
+    <col min="10" max="10" width="60.1719" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.35156" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1701,571 +1782,575 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" t="s" s="4">
+      <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" ht="20.25" customHeight="1">
+      <c r="A3" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="E2" t="s" s="4">
+      <c r="B3" t="s" s="6">
         <v>3</v>
       </c>
-      <c r="F2" t="s" s="4">
+      <c r="C3" t="s" s="7">
         <v>4</v>
       </c>
-      <c r="G2" t="s" s="4">
+      <c r="D3" t="s" s="7">
         <v>5</v>
       </c>
-      <c r="H2" t="s" s="4">
+      <c r="E3" t="s" s="7">
         <v>6</v>
       </c>
-      <c r="I2" t="s" s="4">
+      <c r="F3" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="J2" t="s" s="4">
+      <c r="G3" t="s" s="7">
         <v>8</v>
       </c>
-      <c r="K2" t="s" s="4">
+      <c r="H3" t="s" s="7">
         <v>9</v>
       </c>
+      <c r="I3" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s" s="7">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" ht="248.25" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7">
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="D3" t="s" s="8">
+      <c r="B4" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s" s="10">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s" s="10">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s" s="10">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="8">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s" s="9">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s" s="10">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s" s="10">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s" s="10">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s" s="10">
+        <v>30</v>
+      </c>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s" s="10">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s" s="10">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s" s="10">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s" s="10">
+        <v>37</v>
+      </c>
+      <c r="I6" t="s" s="10">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s" s="10">
+        <v>39</v>
+      </c>
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="8">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s" s="9">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s" s="10">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s" s="10">
+        <v>44</v>
+      </c>
+      <c r="G7" t="s" s="10">
+        <v>45</v>
+      </c>
+      <c r="H7" t="s" s="10">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s" s="10">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s" s="10">
+        <v>48</v>
+      </c>
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s" s="9">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s" s="10">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s" s="10">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s" s="10">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s" s="10">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s" s="10">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s" s="10">
+        <v>55</v>
+      </c>
+      <c r="I8" t="s" s="10">
+        <v>56</v>
+      </c>
+      <c r="J8" t="s" s="10">
+        <v>57</v>
+      </c>
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="8">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s" s="9">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s" s="10">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s" s="10">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s" s="10">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s" s="10">
+        <v>62</v>
+      </c>
+      <c r="G9" t="s" s="10">
+        <v>63</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" t="s" s="10">
+        <v>64</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="8">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s" s="9">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s" s="10">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s" s="10">
+        <v>67</v>
+      </c>
+      <c r="E10" t="s" s="10">
+        <v>68</v>
+      </c>
+      <c r="F10" t="s" s="10">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s" s="10">
+        <v>70</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" t="s" s="10">
+        <v>71</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="8">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s" s="9">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s" s="10">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s" s="10">
+        <v>74</v>
+      </c>
+      <c r="E11" t="s" s="10">
+        <v>75</v>
+      </c>
+      <c r="F11" t="s" s="10">
+        <v>76</v>
+      </c>
+      <c r="G11" t="s" s="10">
+        <v>77</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" t="s" s="10">
+        <v>78</v>
+      </c>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="8">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s" s="9">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s" s="10">
+        <v>80</v>
+      </c>
+      <c r="D12" t="s" s="10">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s" s="10">
+        <v>82</v>
+      </c>
+      <c r="F12" t="s" s="10">
+        <v>83</v>
+      </c>
+      <c r="G12" t="s" s="10">
+        <v>84</v>
+      </c>
+      <c r="H12" t="s" s="10">
+        <v>85</v>
+      </c>
+      <c r="I12" t="s" s="10">
+        <v>86</v>
+      </c>
+      <c r="J12" t="s" s="10">
+        <v>87</v>
+      </c>
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="8">
         <v>10</v>
       </c>
-      <c r="E3" t="s" s="8">
+      <c r="B13" t="s" s="9">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s" s="10">
+        <v>89</v>
+      </c>
+      <c r="D13" t="s" s="10">
+        <v>90</v>
+      </c>
+      <c r="E13" t="s" s="10">
+        <v>91</v>
+      </c>
+      <c r="F13" t="s" s="10">
+        <v>92</v>
+      </c>
+      <c r="G13" t="s" s="10">
+        <v>93</v>
+      </c>
+      <c r="H13" t="s" s="10">
+        <v>94</v>
+      </c>
+      <c r="I13" t="s" s="10">
+        <v>95</v>
+      </c>
+      <c r="J13" t="s" s="10">
+        <v>96</v>
+      </c>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" s="8">
         <v>11</v>
       </c>
-      <c r="F3" t="s" s="8">
+      <c r="B14" t="s" s="9">
+        <v>97</v>
+      </c>
+      <c r="C14" t="s" s="10">
+        <v>98</v>
+      </c>
+      <c r="D14" t="s" s="10">
+        <v>99</v>
+      </c>
+      <c r="E14" t="s" s="10">
+        <v>100</v>
+      </c>
+      <c r="F14" t="s" s="10">
+        <v>101</v>
+      </c>
+      <c r="G14" t="s" s="10">
+        <v>102</v>
+      </c>
+      <c r="H14" t="s" s="10">
+        <v>103</v>
+      </c>
+      <c r="I14" t="s" s="10">
+        <v>104</v>
+      </c>
+      <c r="J14" t="s" s="10">
+        <v>105</v>
+      </c>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" s="8">
         <v>12</v>
       </c>
-      <c r="G3" t="s" s="8">
+      <c r="B15" t="s" s="9">
+        <v>106</v>
+      </c>
+      <c r="C15" t="s" s="10">
+        <v>107</v>
+      </c>
+      <c r="D15" t="s" s="10">
+        <v>108</v>
+      </c>
+      <c r="E15" t="s" s="10">
+        <v>109</v>
+      </c>
+      <c r="F15" t="s" s="10">
+        <v>110</v>
+      </c>
+      <c r="G15" t="s" s="10">
+        <v>111</v>
+      </c>
+      <c r="H15" t="s" s="10">
+        <v>112</v>
+      </c>
+      <c r="I15" t="s" s="10">
+        <v>113</v>
+      </c>
+      <c r="J15" t="s" s="10">
+        <v>114</v>
+      </c>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" s="8">
         <v>13</v>
       </c>
-      <c r="H3" t="s" s="8">
+      <c r="B16" t="s" s="9">
+        <v>115</v>
+      </c>
+      <c r="C16" t="s" s="10">
+        <v>116</v>
+      </c>
+      <c r="D16" t="s" s="10">
+        <v>117</v>
+      </c>
+      <c r="E16" t="s" s="10">
+        <v>118</v>
+      </c>
+      <c r="F16" t="s" s="10">
+        <v>119</v>
+      </c>
+      <c r="G16" t="s" s="10">
+        <v>120</v>
+      </c>
+      <c r="H16" t="s" s="10">
+        <v>121</v>
+      </c>
+      <c r="I16" t="s" s="10">
+        <v>122</v>
+      </c>
+      <c r="J16" t="s" s="10">
+        <v>123</v>
+      </c>
+      <c r="K16" t="s" s="10">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" s="8">
         <v>14</v>
       </c>
-      <c r="I3" t="s" s="8">
+      <c r="B17" t="s" s="9">
+        <v>125</v>
+      </c>
+      <c r="C17" t="s" s="10">
+        <v>126</v>
+      </c>
+      <c r="D17" t="s" s="10">
+        <v>127</v>
+      </c>
+      <c r="E17" t="s" s="10">
+        <v>128</v>
+      </c>
+      <c r="F17" t="s" s="10">
+        <v>129</v>
+      </c>
+      <c r="G17" t="s" s="10">
+        <v>130</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" t="s" s="10">
+        <v>131</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="K17" t="s" s="10">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" s="8">
         <v>15</v>
       </c>
-      <c r="J3" t="s" s="8">
-        <v>16</v>
-      </c>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" ht="248.05" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s" s="13">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s" s="13">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s" s="13">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s" s="13">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s" s="13">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s" s="13">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s" s="13">
-        <v>23</v>
-      </c>
-      <c r="K4" s="14"/>
-    </row>
-    <row r="5" ht="236.05" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s" s="13">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s" s="13">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s" s="13">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s" s="13">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s" s="13">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s" s="13">
-        <v>29</v>
-      </c>
-      <c r="J5" t="s" s="13">
-        <v>30</v>
-      </c>
-      <c r="K5" s="14"/>
-    </row>
-    <row r="6" ht="332.05" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s" s="13">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s" s="13">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s" s="13">
-        <v>34</v>
-      </c>
-      <c r="H6" t="s" s="13">
-        <v>35</v>
-      </c>
-      <c r="I6" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="J6" t="s" s="13">
-        <v>37</v>
-      </c>
-      <c r="K6" s="14"/>
-    </row>
-    <row r="7" ht="368.05" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s" s="13">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s" s="13">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s" s="13">
-        <v>40</v>
-      </c>
-      <c r="G7" t="s" s="13">
-        <v>41</v>
-      </c>
-      <c r="H7" t="s" s="13">
-        <v>42</v>
-      </c>
-      <c r="I7" t="s" s="13">
-        <v>43</v>
-      </c>
-      <c r="J7" t="s" s="13">
-        <v>44</v>
-      </c>
-      <c r="K7" s="14"/>
-    </row>
-    <row r="8" ht="284.05" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s" s="13">
-        <v>45</v>
-      </c>
-      <c r="E8" t="s" s="13">
-        <v>46</v>
-      </c>
-      <c r="F8" t="s" s="13">
-        <v>47</v>
-      </c>
-      <c r="G8" t="s" s="13">
-        <v>48</v>
-      </c>
-      <c r="H8" t="s" s="13">
-        <v>49</v>
-      </c>
-      <c r="I8" t="s" s="13">
-        <v>50</v>
-      </c>
-      <c r="J8" t="s" s="13">
-        <v>51</v>
-      </c>
-      <c r="K8" s="14"/>
-    </row>
-    <row r="9" ht="284.05" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s" s="13">
-        <v>52</v>
-      </c>
-      <c r="E9" t="s" s="13">
-        <v>53</v>
-      </c>
-      <c r="F9" t="s" s="13">
-        <v>54</v>
-      </c>
-      <c r="G9" t="s" s="13">
-        <v>55</v>
-      </c>
-      <c r="H9" t="s" s="13">
-        <v>56</v>
-      </c>
-      <c r="I9" t="s" s="13">
-        <v>57</v>
-      </c>
-      <c r="J9" t="s" s="13">
-        <v>58</v>
-      </c>
-      <c r="K9" s="14"/>
-    </row>
-    <row r="10" ht="200.05" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s" s="13">
-        <v>59</v>
-      </c>
-      <c r="E10" t="s" s="13">
-        <v>60</v>
-      </c>
-      <c r="F10" t="s" s="13">
-        <v>61</v>
-      </c>
-      <c r="G10" t="s" s="13">
-        <v>62</v>
-      </c>
-      <c r="H10" t="s" s="13">
-        <v>63</v>
-      </c>
-      <c r="I10" t="s" s="13">
-        <v>64</v>
-      </c>
-      <c r="J10" t="s" s="13">
-        <v>65</v>
-      </c>
-      <c r="K10" s="14"/>
-    </row>
-    <row r="11" ht="224.05" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s" s="13">
-        <v>66</v>
-      </c>
-      <c r="E11" t="s" s="13">
-        <v>67</v>
-      </c>
-      <c r="F11" t="s" s="13">
-        <v>68</v>
-      </c>
-      <c r="G11" t="s" s="13">
-        <v>69</v>
-      </c>
-      <c r="H11" t="s" s="13">
-        <v>70</v>
-      </c>
-      <c r="I11" t="s" s="13">
-        <v>71</v>
-      </c>
-      <c r="J11" t="s" s="13">
-        <v>72</v>
-      </c>
-      <c r="K11" s="14"/>
-    </row>
-    <row r="12" ht="296.05" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s" s="13">
-        <v>73</v>
-      </c>
-      <c r="E12" t="s" s="13">
-        <v>74</v>
-      </c>
-      <c r="F12" t="s" s="13">
-        <v>75</v>
-      </c>
-      <c r="G12" t="s" s="13">
-        <v>76</v>
-      </c>
-      <c r="H12" t="s" s="13">
-        <v>77</v>
-      </c>
-      <c r="I12" t="s" s="13">
-        <v>78</v>
-      </c>
-      <c r="J12" t="s" s="13">
-        <v>79</v>
-      </c>
-      <c r="K12" s="14"/>
-    </row>
-    <row r="13" ht="248.05" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s" s="13">
-        <v>80</v>
-      </c>
-      <c r="E13" t="s" s="13">
-        <v>81</v>
-      </c>
-      <c r="F13" t="s" s="13">
-        <v>82</v>
-      </c>
-      <c r="G13" t="s" s="13">
-        <v>83</v>
-      </c>
-      <c r="H13" t="s" s="13">
-        <v>84</v>
-      </c>
-      <c r="I13" t="s" s="13">
-        <v>85</v>
-      </c>
-      <c r="J13" t="s" s="13">
-        <v>86</v>
-      </c>
-      <c r="K13" s="14"/>
-    </row>
-    <row r="14" ht="224.05" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s" s="13">
-        <v>87</v>
-      </c>
-      <c r="E14" t="s" s="13">
-        <v>88</v>
-      </c>
-      <c r="F14" t="s" s="13">
-        <v>89</v>
-      </c>
-      <c r="G14" t="s" s="13">
-        <v>90</v>
-      </c>
-      <c r="H14" t="s" s="13">
-        <v>91</v>
-      </c>
-      <c r="I14" t="s" s="13">
-        <v>92</v>
-      </c>
-      <c r="J14" t="s" s="13">
-        <v>93</v>
-      </c>
-      <c r="K14" s="14"/>
-    </row>
-    <row r="15" ht="344.05" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s" s="13">
-        <v>94</v>
-      </c>
-      <c r="E15" t="s" s="13">
-        <v>95</v>
-      </c>
-      <c r="F15" t="s" s="13">
-        <v>96</v>
-      </c>
-      <c r="G15" t="s" s="13">
-        <v>97</v>
-      </c>
-      <c r="H15" t="s" s="13">
-        <v>98</v>
-      </c>
-      <c r="I15" t="s" s="13">
-        <v>99</v>
-      </c>
-      <c r="J15" t="s" s="13">
-        <v>100</v>
-      </c>
-      <c r="K15" s="14"/>
-    </row>
-    <row r="16" ht="248.05" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s" s="13">
-        <v>101</v>
-      </c>
-      <c r="E16" t="s" s="13">
-        <v>102</v>
-      </c>
-      <c r="F16" t="s" s="13">
-        <v>103</v>
-      </c>
-      <c r="G16" t="s" s="13">
-        <v>104</v>
-      </c>
-      <c r="H16" t="s" s="13">
-        <v>105</v>
-      </c>
-      <c r="I16" t="s" s="13">
-        <v>106</v>
-      </c>
-      <c r="J16" t="s" s="13">
-        <v>107</v>
-      </c>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" ht="284.05" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s" s="13">
-        <v>108</v>
-      </c>
-      <c r="E17" t="s" s="13">
-        <v>109</v>
-      </c>
-      <c r="F17" t="s" s="13">
-        <v>110</v>
-      </c>
-      <c r="G17" t="s" s="13">
-        <v>111</v>
-      </c>
-      <c r="H17" t="s" s="13">
-        <v>112</v>
-      </c>
-      <c r="I17" t="s" s="13">
-        <v>113</v>
-      </c>
-      <c r="J17" t="s" s="13">
-        <v>114</v>
-      </c>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" ht="272.05" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12">
-        <v>16</v>
-      </c>
-      <c r="D18" t="s" s="13">
-        <v>115</v>
-      </c>
-      <c r="E18" t="s" s="13">
-        <v>116</v>
-      </c>
-      <c r="F18" t="s" s="13">
-        <v>117</v>
-      </c>
-      <c r="G18" t="s" s="13">
-        <v>118</v>
-      </c>
-      <c r="H18" t="s" s="13">
-        <v>119</v>
-      </c>
-      <c r="I18" t="s" s="13">
-        <v>120</v>
-      </c>
-      <c r="J18" t="s" s="13">
-        <v>121</v>
-      </c>
-      <c r="K18" s="14"/>
+      <c r="B18" t="s" s="9">
+        <v>133</v>
+      </c>
+      <c r="C18" t="s" s="10">
+        <v>134</v>
+      </c>
+      <c r="D18" t="s" s="10">
+        <v>135</v>
+      </c>
+      <c r="E18" t="s" s="10">
+        <v>136</v>
+      </c>
+      <c r="F18" t="s" s="10">
+        <v>137</v>
+      </c>
+      <c r="G18" t="s" s="10">
+        <v>138</v>
+      </c>
+      <c r="H18" t="s" s="10">
+        <v>139</v>
+      </c>
+      <c r="I18" t="s" s="10">
+        <v>140</v>
+      </c>
+      <c r="J18" t="s" s="10">
+        <v>141</v>
+      </c>
+      <c r="K18" t="s" s="10">
+        <v>142</v>
+      </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
+      <c r="A19" s="8">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s" s="9">
+        <v>143</v>
+      </c>
+      <c r="C19" t="s" s="10">
+        <v>144</v>
+      </c>
+      <c r="D19" t="s" s="10">
+        <v>145</v>
+      </c>
+      <c r="E19" t="s" s="10">
+        <v>146</v>
+      </c>
+      <c r="F19" t="s" s="10">
+        <v>147</v>
+      </c>
+      <c r="G19" t="s" s="10">
+        <v>148</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" t="s" s="10">
+        <v>149</v>
+      </c>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>